<commit_message>
Fix stroop, remove clock drawing
</commit_message>
<xml_diff>
--- a/blank.xlsx
+++ b/blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/prut/Documents/superAI2024/Level3/rule-based/neuropsychological/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12F1AA92-2AEF-A140-8F3D-8E54F695CB73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B6DFE15-D6A6-EF43-BAF1-5A6951B95914}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19540" tabRatio="738" xr2:uid="{621A9CD4-A382-6048-B97E-33F5B9C8B8FF}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="38080" windowHeight="19540" tabRatio="738" activeTab="6" xr2:uid="{621A9CD4-A382-6048-B97E-33F5B9C8B8FF}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="15" r:id="rId1"/>
@@ -2343,10 +2343,16 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2380,33 +2386,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -2416,10 +2395,31 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2732,7 +2732,7 @@
   </sheetPr>
   <dimension ref="B1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
@@ -13058,15 +13058,15 @@
       <c r="B5" s="119"/>
     </row>
     <row r="6" spans="2:9" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="182" t="s">
+      <c r="B6" s="184" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="183"/>
-      <c r="D6" s="183"/>
-      <c r="E6" s="183"/>
-      <c r="F6" s="183"/>
-      <c r="G6" s="183"/>
-      <c r="H6" s="184"/>
+      <c r="C6" s="185"/>
+      <c r="D6" s="185"/>
+      <c r="E6" s="185"/>
+      <c r="F6" s="185"/>
+      <c r="G6" s="185"/>
+      <c r="H6" s="186"/>
     </row>
     <row r="7" spans="2:9" ht="24" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="97" t="s">
@@ -13176,12 +13176,12 @@
       <c r="B14" s="173" t="s">
         <v>3</v>
       </c>
-      <c r="C14" s="185"/>
-      <c r="D14" s="185"/>
-      <c r="E14" s="185"/>
-      <c r="F14" s="185"/>
-      <c r="G14" s="185"/>
-      <c r="H14" s="186"/>
+      <c r="C14" s="187"/>
+      <c r="D14" s="187"/>
+      <c r="E14" s="187"/>
+      <c r="F14" s="187"/>
+      <c r="G14" s="187"/>
+      <c r="H14" s="188"/>
     </row>
     <row r="15" spans="2:9" ht="27" x14ac:dyDescent="0.45">
       <c r="B15" s="124"/>
@@ -13264,15 +13264,15 @@
     </row>
     <row r="19" spans="2:9" ht="20" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="20" spans="2:9" ht="28" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="187" t="s">
+      <c r="B20" s="189" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="188"/>
-      <c r="D20" s="188"/>
-      <c r="E20" s="188"/>
-      <c r="F20" s="188"/>
-      <c r="G20" s="188"/>
-      <c r="H20" s="189"/>
+      <c r="C20" s="190"/>
+      <c r="D20" s="190"/>
+      <c r="E20" s="190"/>
+      <c r="F20" s="190"/>
+      <c r="G20" s="190"/>
+      <c r="H20" s="191"/>
     </row>
     <row r="21" spans="2:9" ht="27" x14ac:dyDescent="0.45">
       <c r="B21" s="133"/>
@@ -13357,77 +13357,77 @@
       <c r="H26" s="120"/>
     </row>
     <row r="27" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="190" t="s">
+      <c r="B27" s="192" t="s">
         <v>179</v>
       </c>
-      <c r="C27" s="191"/>
-      <c r="D27" s="191"/>
-      <c r="E27" s="191"/>
-      <c r="F27" s="191"/>
-      <c r="G27" s="191"/>
-      <c r="H27" s="192"/>
+      <c r="C27" s="193"/>
+      <c r="D27" s="193"/>
+      <c r="E27" s="193"/>
+      <c r="F27" s="193"/>
+      <c r="G27" s="193"/>
+      <c r="H27" s="194"/>
       <c r="I27" s="139"/>
     </row>
     <row r="28" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="178" t="s">
+      <c r="B28" s="180" t="s">
         <v>249</v>
       </c>
-      <c r="C28" s="179"/>
-      <c r="D28" s="179"/>
-      <c r="E28" s="180" t="s">
+      <c r="C28" s="178"/>
+      <c r="D28" s="178"/>
+      <c r="E28" s="181" t="s">
         <v>253</v>
       </c>
-      <c r="F28" s="179"/>
-      <c r="G28" s="179"/>
-      <c r="H28" s="181"/>
+      <c r="F28" s="178"/>
+      <c r="G28" s="178"/>
+      <c r="H28" s="179"/>
     </row>
     <row r="29" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B29" s="178" t="s">
+      <c r="B29" s="180" t="s">
         <v>250</v>
       </c>
-      <c r="C29" s="179"/>
-      <c r="D29" s="179"/>
-      <c r="E29" s="180" t="s">
+      <c r="C29" s="178"/>
+      <c r="D29" s="178"/>
+      <c r="E29" s="181" t="s">
         <v>254</v>
       </c>
-      <c r="F29" s="179"/>
-      <c r="G29" s="179"/>
-      <c r="H29" s="181"/>
+      <c r="F29" s="178"/>
+      <c r="G29" s="178"/>
+      <c r="H29" s="179"/>
     </row>
     <row r="30" spans="2:9" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B30" s="178" t="s">
+      <c r="B30" s="180" t="s">
         <v>251</v>
       </c>
-      <c r="C30" s="179"/>
-      <c r="D30" s="179"/>
-      <c r="E30" s="193" t="s">
+      <c r="C30" s="178"/>
+      <c r="D30" s="178"/>
+      <c r="E30" s="182" t="s">
         <v>255</v>
       </c>
-      <c r="F30" s="193"/>
-      <c r="G30" s="193"/>
-      <c r="H30" s="194"/>
+      <c r="F30" s="182"/>
+      <c r="G30" s="182"/>
+      <c r="H30" s="183"/>
     </row>
     <row r="31" spans="2:9" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B31" s="178" t="s">
+      <c r="B31" s="180" t="s">
         <v>252</v>
       </c>
-      <c r="C31" s="180"/>
-      <c r="D31" s="180"/>
-      <c r="E31" s="193" t="s">
+      <c r="C31" s="181"/>
+      <c r="D31" s="181"/>
+      <c r="E31" s="182" t="s">
         <v>256</v>
       </c>
-      <c r="F31" s="193"/>
-      <c r="G31" s="193"/>
-      <c r="H31" s="194"/>
+      <c r="F31" s="182"/>
+      <c r="G31" s="182"/>
+      <c r="H31" s="183"/>
     </row>
     <row r="32" spans="2:9" ht="8.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B32" s="178"/>
-      <c r="C32" s="179"/>
-      <c r="D32" s="179"/>
-      <c r="E32" s="179"/>
-      <c r="F32" s="179"/>
-      <c r="G32" s="179"/>
-      <c r="H32" s="181"/>
+      <c r="B32" s="180"/>
+      <c r="C32" s="178"/>
+      <c r="D32" s="178"/>
+      <c r="E32" s="178"/>
+      <c r="F32" s="178"/>
+      <c r="G32" s="178"/>
+      <c r="H32" s="179"/>
     </row>
     <row r="33" spans="2:8" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="140" t="s">
@@ -13591,12 +13591,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="E32:H32"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="E30:H30"/>
-    <mergeCell ref="E31:H31"/>
     <mergeCell ref="B29:D29"/>
     <mergeCell ref="E29:H29"/>
     <mergeCell ref="B6:H6"/>
@@ -13605,6 +13599,12 @@
     <mergeCell ref="B27:H27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="E28:H28"/>
+    <mergeCell ref="E32:H32"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="E30:H30"/>
+    <mergeCell ref="E31:H31"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.56000000000000005" right="0.25" top="0.86" bottom="0.25" header="0.53" footer="0.5"/>
@@ -13681,16 +13681,16 @@
       <c r="B5" s="150"/>
     </row>
     <row r="6" spans="2:9" ht="30" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="202" t="s">
+      <c r="B6" s="195" t="s">
         <v>101</v>
       </c>
-      <c r="C6" s="203"/>
-      <c r="D6" s="203"/>
-      <c r="E6" s="204"/>
+      <c r="C6" s="196"/>
+      <c r="D6" s="196"/>
+      <c r="E6" s="197"/>
     </row>
     <row r="7" spans="2:9" ht="27" x14ac:dyDescent="0.45">
-      <c r="B7" s="205"/>
-      <c r="C7" s="206"/>
+      <c r="B7" s="202"/>
+      <c r="C7" s="203"/>
       <c r="D7" s="18" t="s">
         <v>13</v>
       </c>
@@ -13699,39 +13699,39 @@
       </c>
     </row>
     <row r="8" spans="2:9" ht="20" x14ac:dyDescent="0.3">
-      <c r="B8" s="196" t="s">
+      <c r="B8" s="200" t="s">
         <v>52</v>
       </c>
-      <c r="C8" s="197"/>
+      <c r="C8" s="201"/>
       <c r="D8" s="152" t="s">
         <v>229</v>
       </c>
       <c r="E8" s="153"/>
     </row>
     <row r="9" spans="2:9" ht="20" x14ac:dyDescent="0.3">
-      <c r="B9" s="196" t="s">
+      <c r="B9" s="200" t="s">
         <v>53</v>
       </c>
-      <c r="C9" s="197"/>
+      <c r="C9" s="201"/>
       <c r="D9" s="152" t="s">
         <v>229</v>
       </c>
       <c r="E9" s="153"/>
     </row>
     <row r="10" spans="2:9" ht="20" x14ac:dyDescent="0.3">
-      <c r="B10" s="196" t="s">
+      <c r="B10" s="200" t="s">
         <v>57</v>
       </c>
-      <c r="C10" s="197"/>
+      <c r="C10" s="201"/>
       <c r="E10" s="154" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="11" spans="2:9" ht="20" x14ac:dyDescent="0.3">
-      <c r="B11" s="196" t="s">
+      <c r="B11" s="200" t="s">
         <v>54</v>
       </c>
-      <c r="C11" s="197"/>
+      <c r="C11" s="201"/>
       <c r="D11" s="152" t="s">
         <v>229</v>
       </c>
@@ -13765,20 +13765,20 @@
       </c>
     </row>
     <row r="15" spans="2:9" ht="20" x14ac:dyDescent="0.3">
-      <c r="B15" s="196" t="s">
+      <c r="B15" s="200" t="s">
         <v>55</v>
       </c>
-      <c r="C15" s="197"/>
+      <c r="C15" s="201"/>
       <c r="D15" s="152" t="s">
         <v>229</v>
       </c>
       <c r="E15" s="153"/>
     </row>
     <row r="16" spans="2:9" ht="20" x14ac:dyDescent="0.3">
-      <c r="B16" s="196" t="s">
+      <c r="B16" s="200" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="197"/>
+      <c r="C16" s="201"/>
       <c r="D16" s="152" t="e">
         <f>D8+D9+D11+D15</f>
         <v>#VALUE!</v>
@@ -13786,19 +13786,25 @@
       <c r="E16" s="153"/>
     </row>
     <row r="17" spans="2:5" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="200"/>
-      <c r="C17" s="201"/>
+      <c r="B17" s="205"/>
+      <c r="C17" s="206"/>
       <c r="D17" s="155"/>
       <c r="E17" s="156"/>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="195"/>
-      <c r="C18" s="195"/>
+      <c r="B18" s="204"/>
+      <c r="C18" s="204"/>
       <c r="D18" s="157"/>
       <c r="E18" s="157"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B17:C17"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B8:C8"/>
@@ -13806,12 +13812,6 @@
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B17:C17"/>
   </mergeCells>
   <phoneticPr fontId="0" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13829,8 +13829,8 @@
   </sheetPr>
   <dimension ref="A1:F68"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -14810,7 +14810,7 @@
       </c>
       <c r="E39" t="str">
         <f>IF(NOT(ISNUMBER(Interpretation!D39)), "Invalid Input",
-IF(Interpretation!D39&lt;0.5, "Impaired", "Preserved"))</f>
+IF(Interpretation!D39&gt;0.5, "Impaired", "Preserved"))</f>
         <v>Invalid Input</v>
       </c>
       <c r="F39" s="77">

</xml_diff>